<commit_message>
1. UI adjust 2. Excel report
</commit_message>
<xml_diff>
--- a/report_template/yearly_report.xlsx
+++ b/report_template/yearly_report.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\webApp\AQM\report_template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="14940" windowHeight="9675"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100"/>
   </bookViews>
   <sheets>
     <sheet name="監測年報表" sheetId="1" r:id="rId1"/>
     <sheet name="工作表2" sheetId="2" r:id="rId2"/>
     <sheet name="工作表3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>監測年報表</t>
   </si>
@@ -80,18 +85,6 @@
 UG/M3</t>
   </si>
   <si>
-    <t>周界PM2.5_x000D_
-UG/M3</t>
-  </si>
-  <si>
-    <t>氨_x000D_
-ppb</t>
-  </si>
-  <si>
-    <t>總硫_x000D_
-ppb</t>
-  </si>
-  <si>
     <t>風速_x000D_
 m/s</t>
   </si>
@@ -116,30 +109,6 @@
 mm/h</t>
   </si>
   <si>
-    <t>104/01</t>
-  </si>
-  <si>
-    <t>104/02</t>
-  </si>
-  <si>
-    <t>104/03</t>
-  </si>
-  <si>
-    <t>104/04</t>
-  </si>
-  <si>
-    <t>104/05</t>
-  </si>
-  <si>
-    <t>104/06</t>
-  </si>
-  <si>
-    <t>104/07</t>
-  </si>
-  <si>
-    <t>104/12</t>
-  </si>
-  <si>
     <t>平均值</t>
   </si>
   <si>
@@ -150,18 +119,6 @@
   </si>
   <si>
     <t>內控值</t>
-  </si>
-  <si>
-    <t>有效率(%)</t>
-  </si>
-  <si>
-    <t>限值標準</t>
-  </si>
-  <si>
-    <t>－</t>
-  </si>
-  <si>
-    <t>逾限次數</t>
   </si>
   <si>
     <t>說明</t>
@@ -175,13 +132,65 @@
   <si>
     <t>不可抗力</t>
   </si>
+  <si>
+    <t>1月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有效率(%)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="##0.00"/>
+    <numFmt numFmtId="176" formatCode="0.00_ ;[Red]\-0.00\ "/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -215,7 +224,7 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,6 +240,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0000FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -268,17 +283,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -292,13 +298,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="176" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -307,11 +319,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -322,6 +337,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -361,7 +379,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -375,7 +392,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測年報表!$P$4</c:f>
+              <c:f>監測年報表!$M$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -403,34 +420,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$P$5:$P$12</c:f>
+              <c:f>監測年報表!$M$5:$M$13</c:f>
               <c:numCache>
-                <c:formatCode>##0.00</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>5.8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.82</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.44</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.83</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.57999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.33</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.78</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
+                <c:ptCount val="9"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -446,8 +439,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="70417024"/>
-        <c:axId val="70427008"/>
+        <c:axId val="276981640"/>
+        <c:axId val="276985952"/>
       </c:lineChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -457,7 +450,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測年報表!$Q$4</c:f>
+              <c:f>監測年報表!$N$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -478,34 +471,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>監測年報表!$Q$5:$Q$12</c:f>
+              <c:f>監測年報表!$N$5:$N$13</c:f>
               <c:numCache>
-                <c:formatCode>##0.00</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>2.56</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.84</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.23</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>346.33</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>213.42</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>202.31</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>257.77</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
+                <c:ptCount val="9"/>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -519,11 +488,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="78433280"/>
-        <c:axId val="78430592"/>
+        <c:axId val="276988304"/>
+        <c:axId val="276983600"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="70417024"/>
+        <c:axId val="276981640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -545,13 +514,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70427008"/>
+        <c:crossAx val="276985952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -559,7 +527,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70427008"/>
+        <c:axId val="276985952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -582,19 +550,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="##0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00_ ;[Red]\-0.00\ " sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70417024"/>
+        <c:crossAx val="276981640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="78430592"/>
+        <c:axId val="276983600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="360"/>
@@ -615,7 +582,6 @@
                   <a:rPr lang="zh-TW" altLang="en-US" sz="1000"/>
                   <a:t>風向</a:t>
                 </a:r>
-                <a:endParaRPr altLang="en-US" sz="1000"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -625,13 +591,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78433280"/>
+        <c:crossAx val="276988304"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="90"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="78433280"/>
+        <c:axId val="276988304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -640,13 +606,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78430592"/>
+        <c:crossAx val="276983600"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -761,34 +727,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$B$5:$B$12</c:f>
+              <c:f>監測年報表!$B$5:$B$13</c:f>
               <c:numCache>
-                <c:formatCode>##0.00</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>5.12</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.95</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.1500000000000004</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.22</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.61</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.42</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.52</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
+                <c:ptCount val="9"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -799,7 +741,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測年報表!$X$4</c:f>
+              <c:f>監測年報表!$U$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -821,10 +763,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$X$5:$X$12</c:f>
+              <c:f>監測年報表!$U$5:$U$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -846,7 +788,7 @@
                 <c:pt idx="6">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
@@ -864,8 +806,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="68362240"/>
-        <c:axId val="68363776"/>
+        <c:axId val="276984776"/>
+        <c:axId val="276985168"/>
       </c:lineChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -875,7 +817,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測年報表!$Q$4</c:f>
+              <c:f>監測年報表!$N$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -896,34 +838,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>監測年報表!$Q$5:$Q$12</c:f>
+              <c:f>監測年報表!$N$5:$N$13</c:f>
               <c:numCache>
-                <c:formatCode>##0.00</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>2.56</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.84</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.23</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>346.33</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>213.42</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>202.31</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>257.77</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
+                <c:ptCount val="9"/>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -937,11 +855,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="94992256"/>
-        <c:axId val="94989312"/>
+        <c:axId val="276980856"/>
+        <c:axId val="276986344"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="68362240"/>
+        <c:axId val="276984776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -968,7 +886,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68363776"/>
+        <c:crossAx val="276985168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -976,7 +894,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68363776"/>
+        <c:axId val="276985168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1001,16 +919,16 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="##0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00_ ;[Red]\-0.00\ " sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68362240"/>
+        <c:crossAx val="276984776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94989312"/>
+        <c:axId val="276986344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="360"/>
@@ -1031,7 +949,6 @@
                   <a:rPr lang="zh-TW" altLang="en-US" sz="1000"/>
                   <a:t>風向</a:t>
                 </a:r>
-                <a:endParaRPr altLang="en-US" sz="1000"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1041,13 +958,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94992256"/>
+        <c:crossAx val="276980856"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="90"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94992256"/>
+        <c:axId val="276980856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1056,7 +973,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94989312"/>
+        <c:crossAx val="276986344"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
@@ -1176,34 +1094,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$F$5:$F$12</c:f>
+              <c:f>監測年報表!$F$5:$F$13</c:f>
               <c:numCache>
-                <c:formatCode>##0.00</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.57999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.51</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.43</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.46</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.48</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
+                <c:ptCount val="9"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1214,7 +1108,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測年報表!$Y$4</c:f>
+              <c:f>監測年報表!$V$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1236,10 +1130,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$Y$5:$Y$12</c:f>
+              <c:f>監測年報表!$V$5:$V$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -1261,7 +1155,7 @@
                 <c:pt idx="6">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -1279,8 +1173,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="68383872"/>
-        <c:axId val="68385408"/>
+        <c:axId val="276987520"/>
+        <c:axId val="123574352"/>
       </c:lineChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1290,7 +1184,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測年報表!$Q$4</c:f>
+              <c:f>監測年報表!$N$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1311,34 +1205,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>監測年報表!$Q$5:$Q$12</c:f>
+              <c:f>監測年報表!$N$5:$N$13</c:f>
               <c:numCache>
-                <c:formatCode>##0.00</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>2.56</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.84</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.23</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>346.33</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>213.42</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>202.31</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>257.77</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
+                <c:ptCount val="9"/>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1352,11 +1222,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="95458816"/>
-        <c:axId val="95453568"/>
+        <c:axId val="123573176"/>
+        <c:axId val="123575528"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="68383872"/>
+        <c:axId val="276987520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1383,7 +1253,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68385408"/>
+        <c:crossAx val="123574352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1391,7 +1261,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68385408"/>
+        <c:axId val="123574352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1416,16 +1286,16 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="##0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00_ ;[Red]\-0.00\ " sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68383872"/>
+        <c:crossAx val="276987520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95453568"/>
+        <c:axId val="123575528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="360"/>
@@ -1456,13 +1326,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95458816"/>
+        <c:crossAx val="123573176"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="90"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95458816"/>
+        <c:axId val="123573176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1471,7 +1341,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95453568"/>
+        <c:crossAx val="123575528"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
@@ -1591,34 +1462,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$D$5:$D$12</c:f>
+              <c:f>監測年報表!$D$5:$D$13</c:f>
               <c:numCache>
-                <c:formatCode>##0.00</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>10.61</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.67</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11.1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.95</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.46</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.28</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
+                <c:ptCount val="9"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1629,7 +1476,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測年報表!$Z$4</c:f>
+              <c:f>監測年報表!$W$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1651,10 +1498,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$Z$5:$Z$12</c:f>
+              <c:f>監測年報表!$W$5:$W$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>50</c:v>
                 </c:pt>
@@ -1676,7 +1523,7 @@
                 <c:pt idx="6">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
@@ -1694,8 +1541,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="68409600"/>
-        <c:axId val="68411392"/>
+        <c:axId val="279862008"/>
+        <c:axId val="279858872"/>
       </c:lineChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1705,7 +1552,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測年報表!$Q$4</c:f>
+              <c:f>監測年報表!$N$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1726,34 +1573,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>監測年報表!$Q$5:$Q$12</c:f>
+              <c:f>監測年報表!$N$5:$N$13</c:f>
               <c:numCache>
-                <c:formatCode>##0.00</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>2.56</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.84</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.23</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>346.33</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>213.42</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>202.31</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>257.77</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
+                <c:ptCount val="9"/>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1767,11 +1590,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="95634944"/>
-        <c:axId val="95632000"/>
+        <c:axId val="279857304"/>
+        <c:axId val="279863184"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="68409600"/>
+        <c:axId val="279862008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1798,7 +1621,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68411392"/>
+        <c:crossAx val="279858872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1806,7 +1629,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68411392"/>
+        <c:axId val="279858872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1831,16 +1654,16 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="##0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00_ ;[Red]\-0.00\ " sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68409600"/>
+        <c:crossAx val="279862008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95632000"/>
+        <c:axId val="279863184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="360"/>
@@ -1871,13 +1694,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95634944"/>
+        <c:crossAx val="279857304"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="90"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95634944"/>
+        <c:axId val="279857304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1886,7 +1709,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95632000"/>
+        <c:crossAx val="279863184"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
@@ -2006,34 +1830,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$G$5:$G$12</c:f>
+              <c:f>監測年報表!$G$5:$G$13</c:f>
               <c:numCache>
-                <c:formatCode>##0.00</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>34.659999999999997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>36.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>35.909999999999997</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>36.369999999999997</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>27.21</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16.86</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>29.42</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
+                <c:ptCount val="9"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2044,7 +1844,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測年報表!$AA$4</c:f>
+              <c:f>監測年報表!$X$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2066,10 +1866,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$AA$5:$AA$12</c:f>
+              <c:f>監測年報表!$X$5:$X$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>120</c:v>
                 </c:pt>
@@ -2091,7 +1891,7 @@
                 <c:pt idx="6">
                   <c:v>120</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>120</c:v>
                 </c:pt>
               </c:numCache>
@@ -2109,8 +1909,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="70529024"/>
-        <c:axId val="70530560"/>
+        <c:axId val="279859264"/>
+        <c:axId val="279862792"/>
       </c:lineChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2120,7 +1920,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測年報表!$Q$4</c:f>
+              <c:f>監測年報表!$N$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2141,34 +1941,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>監測年報表!$Q$5:$Q$12</c:f>
+              <c:f>監測年報表!$N$5:$N$13</c:f>
               <c:numCache>
-                <c:formatCode>##0.00</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>2.56</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.84</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.23</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>346.33</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>213.42</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>202.31</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>257.77</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
+                <c:ptCount val="9"/>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2182,11 +1958,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="95835648"/>
-        <c:axId val="95830400"/>
+        <c:axId val="279860048"/>
+        <c:axId val="279859656"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="70529024"/>
+        <c:axId val="279859264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2213,7 +1989,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70530560"/>
+        <c:crossAx val="279862792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2221,7 +1997,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70530560"/>
+        <c:axId val="279862792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2246,16 +2022,16 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="##0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00_ ;[Red]\-0.00\ " sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70529024"/>
+        <c:crossAx val="279859264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95830400"/>
+        <c:axId val="279859656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="360"/>
@@ -2286,13 +2062,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95835648"/>
+        <c:crossAx val="279860048"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="90"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95835648"/>
+        <c:axId val="279860048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2301,7 +2077,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95830400"/>
+        <c:crossAx val="279859656"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
@@ -2433,31 +2210,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$L$5:$L$12</c:f>
+              <c:f>監測年報表!$L$5:$L$13</c:f>
               <c:numCache>
-                <c:formatCode>##0.00</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>72.260000000000005</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>63.05</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>59.8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>55.3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>51.19</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>50.28</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>56.25</c:v>
-                </c:pt>
+                <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
+                <c:ptCount val="9"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2468,7 +2224,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測年報表!$AB$4</c:f>
+              <c:f>監測年報表!$Y$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2490,10 +2246,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$AB$5:$AB$12</c:f>
+              <c:f>監測年報表!$Y$5:$Y$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>125</c:v>
                 </c:pt>
@@ -2515,7 +2271,7 @@
                 <c:pt idx="6">
                   <c:v>125</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>125</c:v>
                 </c:pt>
               </c:numCache>
@@ -2533,8 +2289,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="70550656"/>
-        <c:axId val="70552192"/>
+        <c:axId val="279858480"/>
+        <c:axId val="279860440"/>
       </c:lineChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2544,7 +2300,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測年報表!$Q$4</c:f>
+              <c:f>監測年報表!$N$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2565,34 +2321,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>監測年報表!$Q$5:$Q$12</c:f>
+              <c:f>監測年報表!$N$5:$N$13</c:f>
               <c:numCache>
-                <c:formatCode>##0.00</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>2.56</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.84</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.23</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>346.33</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>213.42</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>202.31</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>257.77</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
+                <c:ptCount val="9"/>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2606,11 +2338,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="95949952"/>
-        <c:axId val="95947008"/>
+        <c:axId val="279856520"/>
+        <c:axId val="279861224"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="70550656"/>
+        <c:axId val="279858480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2637,7 +2369,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70552192"/>
+        <c:crossAx val="279860440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2645,7 +2377,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70552192"/>
+        <c:axId val="279860440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2670,16 +2402,16 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="##0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00_ ;[Red]\-0.00\ " sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70550656"/>
+        <c:crossAx val="279858480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95947008"/>
+        <c:axId val="279861224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="360"/>
@@ -2710,13 +2442,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95949952"/>
+        <c:crossAx val="279856520"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="90"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95949952"/>
+        <c:axId val="279856520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2725,7 +2457,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95947008"/>
+        <c:crossAx val="279861224"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
@@ -2845,34 +2578,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$J$5:$J$12</c:f>
+              <c:f>監測年報表!$J$5:$J$13</c:f>
               <c:numCache>
-                <c:formatCode>##0.00</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0.21</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.22</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.22</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.21</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.17</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.15</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.13</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
+                <c:ptCount val="9"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2883,7 +2592,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測年報表!$AC$4</c:f>
+              <c:f>監測年報表!$Z$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2905,10 +2614,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$AC$5:$AC$12</c:f>
+              <c:f>監測年報表!$Z$5:$Z$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1.5</c:v>
                 </c:pt>
@@ -2930,7 +2639,7 @@
                 <c:pt idx="6">
                   <c:v>1.5</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>1.5</c:v>
                 </c:pt>
               </c:numCache>
@@ -2948,8 +2657,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="70580480"/>
-        <c:axId val="71639040"/>
+        <c:axId val="279856912"/>
+        <c:axId val="279862400"/>
       </c:lineChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2959,7 +2668,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測年報表!$Q$4</c:f>
+              <c:f>監測年報表!$N$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2980,34 +2689,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>監測年報表!$Q$5:$Q$12</c:f>
+              <c:f>監測年報表!$N$5:$N$13</c:f>
               <c:numCache>
-                <c:formatCode>##0.00</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>2.56</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.84</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.23</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>346.33</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>213.42</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>202.31</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>257.77</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
+                <c:ptCount val="9"/>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3021,11 +2706,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="105509248"/>
-        <c:axId val="105506304"/>
+        <c:axId val="279861616"/>
+        <c:axId val="279857696"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="70580480"/>
+        <c:axId val="279856912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3052,7 +2737,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71639040"/>
+        <c:crossAx val="279862400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3060,7 +2745,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71639040"/>
+        <c:axId val="279862400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3085,16 +2770,16 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="##0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00_ ;[Red]\-0.00\ " sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70580480"/>
+        <c:crossAx val="279856912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="105506304"/>
+        <c:axId val="279857696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="360"/>
@@ -3125,13 +2810,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105509248"/>
+        <c:crossAx val="279861616"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="90"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="105509248"/>
+        <c:axId val="279861616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3140,7 +2825,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105506304"/>
+        <c:crossAx val="279857696"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
@@ -3272,31 +2958,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$K$5:$K$12</c:f>
+              <c:f>監測年報表!$K$5:$K$13</c:f>
               <c:numCache>
-                <c:formatCode>##0.00</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>107.45</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>107.55</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>108.35</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>102.42</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>93.85</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>89.14</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>93.23</c:v>
-                </c:pt>
+                <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
+                <c:ptCount val="9"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3307,7 +2972,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測年報表!$AD$4</c:f>
+              <c:f>監測年報表!$AA$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3329,10 +2994,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$AD$5:$AD$12</c:f>
+              <c:f>監測年報表!$AA$5:$AA$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>250</c:v>
                 </c:pt>
@@ -3354,7 +3019,7 @@
                 <c:pt idx="6">
                   <c:v>250</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>250</c:v>
                 </c:pt>
               </c:numCache>
@@ -3372,8 +3037,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="71667072"/>
-        <c:axId val="71672960"/>
+        <c:axId val="279686720"/>
+        <c:axId val="279687504"/>
       </c:lineChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -3383,7 +3048,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>監測年報表!$Q$4</c:f>
+              <c:f>監測年報表!$N$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3404,34 +3069,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>監測年報表!$Q$5:$Q$12</c:f>
+              <c:f>監測年報表!$N$5:$N$13</c:f>
               <c:numCache>
-                <c:formatCode>##0.00</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>2.56</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.84</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.23</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>346.33</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>213.42</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>202.31</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>257.77</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
+                <c:ptCount val="9"/>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3445,11 +3086,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="114019712"/>
-        <c:axId val="114017024"/>
+        <c:axId val="279691424"/>
+        <c:axId val="279687896"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="71667072"/>
+        <c:axId val="279686720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3476,7 +3117,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71672960"/>
+        <c:crossAx val="279687504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3484,7 +3125,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71672960"/>
+        <c:axId val="279687504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3509,16 +3150,16 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="##0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00_ ;[Red]\-0.00\ " sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71667072"/>
+        <c:crossAx val="279686720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="114017024"/>
+        <c:axId val="279687896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="360"/>
@@ -3549,13 +3190,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114019712"/>
+        <c:crossAx val="279691424"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="90"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="114019712"/>
+        <c:axId val="279691424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3564,7 +3205,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114017024"/>
+        <c:crossAx val="279687896"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
@@ -3590,13 +3232,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>838200</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3620,13 +3262,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>838200</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>828675</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3650,13 +3292,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>838200</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:row>99</xdr:row>
       <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3680,13 +3322,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>838200</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>828675</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:row>99</xdr:row>
       <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3710,13 +3352,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>100</xdr:row>
       <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>838200</xdr:colOff>
-      <xdr:row>121</xdr:row>
+      <xdr:row>125</xdr:row>
       <xdr:rowOff>44450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3740,13 +3382,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>838200</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>100</xdr:row>
       <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>828675</xdr:colOff>
-      <xdr:row>121</xdr:row>
+      <xdr:row>125</xdr:row>
       <xdr:rowOff>44450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3770,13 +3412,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>122</xdr:row>
+      <xdr:row>126</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>838200</xdr:colOff>
-      <xdr:row>146</xdr:row>
+      <xdr:row>150</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3800,13 +3442,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>838200</xdr:colOff>
-      <xdr:row>122</xdr:row>
+      <xdr:row>126</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>828675</xdr:colOff>
-      <xdr:row>146</xdr:row>
+      <xdr:row>150</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3872,7 +3514,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3907,7 +3549,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4116,1764 +3758,1310 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD28"/>
+  <dimension ref="A1:AA32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:U1"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="12" width="11.125" customWidth="1"/>
-    <col min="13" max="15" width="11.125" hidden="1" customWidth="1"/>
-    <col min="16" max="30" width="11.125" customWidth="1"/>
+    <col min="1" max="27" width="11.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="4" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="U2" s="4"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="L3" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="4" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="U3" s="4"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:27" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="M4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="N4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="O4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="P4" s="7" t="s">
+      <c r="P4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="Q4" s="7" t="s">
+      <c r="Q4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="R4" s="7" t="s">
+      <c r="R4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="S4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="T4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="U4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD4" s="2" t="s">
-        <v>37</v>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="9">
-        <v>5.12</v>
-      </c>
-      <c r="C5" s="9">
-        <v>14.94</v>
-      </c>
-      <c r="D5" s="9">
-        <v>10.61</v>
-      </c>
-      <c r="E5" s="9">
-        <v>4.33</v>
-      </c>
-      <c r="F5" s="9">
-        <v>0.7</v>
-      </c>
-      <c r="G5" s="9">
-        <v>34.659999999999997</v>
-      </c>
-      <c r="H5" s="9">
-        <v>2.5099999999999998</v>
-      </c>
-      <c r="I5" s="9">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="J5" s="9">
-        <v>0.21</v>
-      </c>
-      <c r="K5" s="9">
-        <v>107.45</v>
-      </c>
-      <c r="L5" s="9">
-        <v>72.260000000000005</v>
-      </c>
+    <row r="5" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
-      <c r="P5" s="9">
-        <v>5.8</v>
-      </c>
-      <c r="Q5" s="9">
-        <v>2.56</v>
-      </c>
-      <c r="R5" s="9">
-        <v>16.82</v>
-      </c>
-      <c r="S5" s="9">
-        <v>76.09</v>
-      </c>
-      <c r="T5" s="9">
-        <v>1019.25</v>
-      </c>
-      <c r="U5" s="9">
-        <v>18</v>
-      </c>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2">
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1">
         <v>20</v>
       </c>
-      <c r="Y5" s="2">
+      <c r="V5" s="1">
         <v>10</v>
       </c>
-      <c r="Z5" s="2">
+      <c r="W5" s="1">
         <v>50</v>
       </c>
-      <c r="AA5" s="2">
+      <c r="X5" s="1">
         <v>120</v>
       </c>
-      <c r="AB5" s="2">
+      <c r="Y5" s="1">
         <v>125</v>
       </c>
-      <c r="AC5" s="2">
+      <c r="Z5" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD5" s="2">
+      <c r="AA5" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="9">
-        <v>3.95</v>
-      </c>
-      <c r="C6" s="9">
-        <v>13.3</v>
-      </c>
-      <c r="D6" s="9">
-        <v>9.67</v>
-      </c>
-      <c r="E6" s="9">
-        <v>3.63</v>
-      </c>
-      <c r="F6" s="9">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="G6" s="9">
-        <v>36.1</v>
-      </c>
-      <c r="H6" s="9">
-        <v>2.44</v>
-      </c>
-      <c r="I6" s="9">
-        <v>2.2200000000000002</v>
-      </c>
-      <c r="J6" s="9">
-        <v>0.22</v>
-      </c>
-      <c r="K6" s="9">
-        <v>107.55</v>
-      </c>
-      <c r="L6" s="9">
-        <v>63.05</v>
-      </c>
+    <row r="6" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
-      <c r="P6" s="9">
-        <v>4.82</v>
-      </c>
-      <c r="Q6" s="9">
-        <v>0.84</v>
-      </c>
-      <c r="R6" s="9">
-        <v>17.64</v>
-      </c>
-      <c r="S6" s="9">
-        <v>79.41</v>
-      </c>
-      <c r="T6" s="9">
-        <v>1018.17</v>
-      </c>
-      <c r="U6" s="9">
-        <v>30.2</v>
-      </c>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2">
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1">
         <v>20</v>
       </c>
-      <c r="Y6" s="2">
+      <c r="V6" s="1">
         <v>10</v>
       </c>
-      <c r="Z6" s="2">
+      <c r="W6" s="1">
         <v>50</v>
       </c>
-      <c r="AA6" s="2">
+      <c r="X6" s="1">
         <v>120</v>
       </c>
-      <c r="AB6" s="2">
+      <c r="Y6" s="1">
         <v>125</v>
       </c>
-      <c r="AC6" s="2">
+      <c r="Z6" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD6" s="2">
+      <c r="AA6" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="9">
-        <v>4.1500000000000004</v>
-      </c>
-      <c r="C7" s="9">
-        <v>14.9</v>
-      </c>
-      <c r="D7" s="9">
-        <v>11.5</v>
-      </c>
-      <c r="E7" s="9">
-        <v>3.4</v>
-      </c>
-      <c r="F7" s="9">
-        <v>0.51</v>
-      </c>
-      <c r="G7" s="9">
-        <v>35.909999999999997</v>
-      </c>
-      <c r="H7" s="9">
-        <v>2.4</v>
-      </c>
-      <c r="I7" s="9">
-        <v>2.19</v>
-      </c>
-      <c r="J7" s="9">
-        <v>0.22</v>
-      </c>
-      <c r="K7" s="9">
-        <v>108.35</v>
-      </c>
-      <c r="L7" s="9">
-        <v>59.8</v>
-      </c>
+    <row r="7" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
-      <c r="P7" s="9">
-        <v>3.44</v>
-      </c>
-      <c r="Q7" s="9">
-        <v>0.23</v>
-      </c>
-      <c r="R7" s="9">
-        <v>20.54</v>
-      </c>
-      <c r="S7" s="9">
-        <v>80.09</v>
-      </c>
-      <c r="T7" s="9">
-        <v>1016.7</v>
-      </c>
-      <c r="U7" s="9">
-        <v>4.8</v>
-      </c>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2">
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1">
         <v>20</v>
       </c>
-      <c r="Y7" s="2">
+      <c r="V7" s="1">
         <v>10</v>
       </c>
-      <c r="Z7" s="2">
+      <c r="W7" s="1">
         <v>50</v>
       </c>
-      <c r="AA7" s="2">
+      <c r="X7" s="1">
         <v>120</v>
       </c>
-      <c r="AB7" s="2">
+      <c r="Y7" s="1">
         <v>125</v>
       </c>
-      <c r="AC7" s="2">
+      <c r="Z7" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD7" s="2">
+      <c r="AA7" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="9">
-        <v>4.22</v>
-      </c>
-      <c r="C8" s="9">
-        <v>14.58</v>
-      </c>
-      <c r="D8" s="9">
-        <v>11.1</v>
-      </c>
-      <c r="E8" s="9">
-        <v>3.48</v>
-      </c>
-      <c r="F8" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="G8" s="9">
-        <v>36.369999999999997</v>
-      </c>
-      <c r="H8" s="9">
-        <v>2.37</v>
-      </c>
-      <c r="I8" s="9">
-        <v>2.15</v>
-      </c>
-      <c r="J8" s="9">
-        <v>0.21</v>
-      </c>
-      <c r="K8" s="9">
-        <v>102.42</v>
-      </c>
-      <c r="L8" s="9">
-        <v>55.3</v>
-      </c>
+    <row r="8" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
-      <c r="P8" s="9">
-        <v>1.83</v>
-      </c>
-      <c r="Q8" s="9">
-        <v>346.33</v>
-      </c>
-      <c r="R8" s="9">
-        <v>23.94</v>
-      </c>
-      <c r="S8" s="9">
-        <v>75.819999999999993</v>
-      </c>
-      <c r="T8" s="9">
-        <v>1013.32</v>
-      </c>
-      <c r="U8" s="9">
-        <v>59</v>
-      </c>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2">
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1">
         <v>20</v>
       </c>
-      <c r="Y8" s="2">
+      <c r="V8" s="1">
         <v>10</v>
       </c>
-      <c r="Z8" s="2">
+      <c r="W8" s="1">
         <v>50</v>
       </c>
-      <c r="AA8" s="2">
+      <c r="X8" s="1">
         <v>120</v>
       </c>
-      <c r="AB8" s="2">
+      <c r="Y8" s="1">
         <v>125</v>
       </c>
-      <c r="AC8" s="2">
+      <c r="Z8" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD8" s="2">
+      <c r="AA8" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="9">
-        <v>3.61</v>
-      </c>
-      <c r="C9" s="9">
-        <v>9.8699999999999992</v>
-      </c>
-      <c r="D9" s="9">
-        <v>6.95</v>
-      </c>
-      <c r="E9" s="9">
-        <v>2.92</v>
-      </c>
-      <c r="F9" s="9">
-        <v>0.43</v>
-      </c>
-      <c r="G9" s="9">
-        <v>27.21</v>
-      </c>
-      <c r="H9" s="9">
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="I9" s="9">
-        <v>2.27</v>
-      </c>
-      <c r="J9" s="9">
-        <v>0.17</v>
-      </c>
-      <c r="K9" s="9">
-        <v>93.85</v>
-      </c>
-      <c r="L9" s="9">
-        <v>51.19</v>
-      </c>
+    <row r="9" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
-      <c r="P9" s="9">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="Q9" s="9">
-        <v>213.42</v>
-      </c>
-      <c r="R9" s="9">
-        <v>27.18</v>
-      </c>
-      <c r="S9" s="9">
-        <v>82.43</v>
-      </c>
-      <c r="T9" s="9">
-        <v>1009.7</v>
-      </c>
-      <c r="U9" s="9">
-        <v>464.6</v>
-      </c>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-      <c r="X9" s="2">
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1">
         <v>20</v>
       </c>
-      <c r="Y9" s="2">
+      <c r="V9" s="1">
         <v>10</v>
       </c>
-      <c r="Z9" s="2">
+      <c r="W9" s="1">
         <v>50</v>
       </c>
-      <c r="AA9" s="2">
+      <c r="X9" s="1">
         <v>120</v>
       </c>
-      <c r="AB9" s="2">
+      <c r="Y9" s="1">
         <v>125</v>
       </c>
-      <c r="AC9" s="2">
+      <c r="Z9" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD9" s="2">
+      <c r="AA9" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="9">
-        <v>4.42</v>
-      </c>
-      <c r="C10" s="9">
-        <v>9.57</v>
-      </c>
-      <c r="D10" s="9">
-        <v>5.46</v>
-      </c>
-      <c r="E10" s="9">
-        <v>4.1100000000000003</v>
-      </c>
-      <c r="F10" s="9">
-        <v>0.46</v>
-      </c>
-      <c r="G10" s="9">
-        <v>16.86</v>
-      </c>
-      <c r="H10" s="9">
-        <v>2.37</v>
-      </c>
-      <c r="I10" s="9">
-        <v>2.2200000000000002</v>
-      </c>
-      <c r="J10" s="9">
-        <v>0.15</v>
-      </c>
-      <c r="K10" s="9">
-        <v>89.14</v>
-      </c>
-      <c r="L10" s="9">
-        <v>50.28</v>
-      </c>
+    <row r="10" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
-      <c r="P10" s="9">
-        <v>2.33</v>
-      </c>
-      <c r="Q10" s="9">
-        <v>202.31</v>
-      </c>
-      <c r="R10" s="9">
-        <v>30.1</v>
-      </c>
-      <c r="S10" s="9">
-        <v>76.64</v>
-      </c>
-      <c r="T10" s="9">
-        <v>1008.31</v>
-      </c>
-      <c r="U10" s="9">
-        <v>1.4</v>
-      </c>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-      <c r="X10" s="2">
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1">
         <v>20</v>
       </c>
-      <c r="Y10" s="2">
+      <c r="V10" s="1">
         <v>10</v>
       </c>
-      <c r="Z10" s="2">
+      <c r="W10" s="1">
         <v>50</v>
       </c>
-      <c r="AA10" s="2">
+      <c r="X10" s="1">
         <v>120</v>
       </c>
-      <c r="AB10" s="2">
+      <c r="Y10" s="1">
         <v>125</v>
       </c>
-      <c r="AC10" s="2">
+      <c r="Z10" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD10" s="2">
+      <c r="AA10" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="9">
-        <v>3.52</v>
-      </c>
-      <c r="C11" s="9">
-        <v>8.0500000000000007</v>
-      </c>
-      <c r="D11" s="9">
-        <v>4.28</v>
-      </c>
-      <c r="E11" s="9">
-        <v>3.76</v>
-      </c>
-      <c r="F11" s="9">
-        <v>0.48</v>
-      </c>
-      <c r="G11" s="9">
-        <v>29.42</v>
-      </c>
-      <c r="H11" s="9">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="I11" s="9">
-        <v>2.16</v>
-      </c>
-      <c r="J11" s="9">
-        <v>0.13</v>
-      </c>
-      <c r="K11" s="9">
-        <v>93.23</v>
-      </c>
-      <c r="L11" s="9">
-        <v>56.25</v>
-      </c>
+    <row r="11" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
-      <c r="P11" s="9">
-        <v>0.78</v>
-      </c>
-      <c r="Q11" s="9">
-        <v>257.77</v>
-      </c>
-      <c r="R11" s="9">
-        <v>29.4</v>
-      </c>
-      <c r="S11" s="9">
-        <v>78.84</v>
-      </c>
-      <c r="T11" s="9">
-        <v>1002.69</v>
-      </c>
-      <c r="U11" s="9">
-        <v>110.4</v>
-      </c>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
-      <c r="X11" s="2">
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1">
         <v>20</v>
       </c>
-      <c r="Y11" s="2">
+      <c r="V11" s="1">
         <v>10</v>
       </c>
-      <c r="Z11" s="2">
+      <c r="W11" s="1">
         <v>50</v>
       </c>
-      <c r="AA11" s="2">
+      <c r="X11" s="1">
         <v>120</v>
       </c>
-      <c r="AB11" s="2">
+      <c r="Y11" s="1">
         <v>125</v>
       </c>
-      <c r="AC11" s="2">
+      <c r="Z11" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD11" s="2">
+      <c r="AA11" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="9">
-        <v>0</v>
-      </c>
-      <c r="C12" s="9">
-        <v>0</v>
-      </c>
-      <c r="D12" s="9">
-        <v>0</v>
-      </c>
-      <c r="E12" s="9">
-        <v>0</v>
-      </c>
-      <c r="F12" s="9">
-        <v>0</v>
-      </c>
-      <c r="G12" s="9">
-        <v>0</v>
-      </c>
-      <c r="H12" s="9">
-        <v>0</v>
-      </c>
-      <c r="I12" s="9">
-        <v>0</v>
-      </c>
-      <c r="J12" s="9">
-        <v>0</v>
-      </c>
+    <row r="12" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
-      <c r="P12" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="9">
-        <v>0</v>
-      </c>
-      <c r="R12" s="9">
-        <v>0</v>
-      </c>
-      <c r="S12" s="9">
-        <v>0</v>
-      </c>
-      <c r="T12" s="9">
-        <v>0</v>
-      </c>
-      <c r="U12" s="9">
-        <v>0</v>
-      </c>
-      <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
-      <c r="X12" s="2">
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+    </row>
+    <row r="13" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1">
         <v>20</v>
       </c>
-      <c r="Y12" s="2">
+      <c r="V13" s="1">
         <v>10</v>
       </c>
-      <c r="Z12" s="2">
+      <c r="W13" s="1">
         <v>50</v>
       </c>
-      <c r="AA12" s="2">
+      <c r="X13" s="1">
         <v>120</v>
       </c>
-      <c r="AB12" s="2">
+      <c r="Y13" s="1">
         <v>125</v>
       </c>
-      <c r="AC12" s="2">
+      <c r="Z13" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD12" s="2">
+      <c r="AA13" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="10">
-        <v>3.6237499999999998</v>
-      </c>
-      <c r="C13" s="10">
-        <v>10.651249999999999</v>
-      </c>
-      <c r="D13" s="10">
-        <v>7.44625</v>
-      </c>
-      <c r="E13" s="10">
-        <v>3.2037499999999999</v>
-      </c>
-      <c r="F13" s="10">
-        <v>0.45750000000000002</v>
-      </c>
-      <c r="G13" s="10">
-        <v>27.06625</v>
-      </c>
-      <c r="H13" s="10">
-        <v>2.1025</v>
-      </c>
-      <c r="I13" s="10">
-        <v>1.93875</v>
-      </c>
-      <c r="J13" s="10">
-        <v>0.16375000000000001</v>
-      </c>
-      <c r="K13" s="10">
-        <v>100.28428571428572</v>
-      </c>
-      <c r="L13" s="10">
-        <v>58.304285714285719</v>
-      </c>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10">
-        <v>2.4474999999999998</v>
-      </c>
-      <c r="Q13" s="10">
-        <v>127.9325</v>
-      </c>
-      <c r="R13" s="10">
-        <v>20.702500000000001</v>
-      </c>
-      <c r="S13" s="10">
-        <v>68.665000000000006</v>
-      </c>
-      <c r="T13" s="10">
-        <v>886.01750000000004</v>
-      </c>
-      <c r="U13" s="10">
-        <v>86.05</v>
-      </c>
-      <c r="V13" s="2"/>
-      <c r="W13" s="2"/>
-      <c r="X13" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y13" s="2">
-        <v>10</v>
-      </c>
-      <c r="Z13" s="2">
-        <v>50</v>
-      </c>
-      <c r="AA13" s="2">
-        <v>120</v>
-      </c>
-      <c r="AB13" s="2">
-        <v>125</v>
-      </c>
-      <c r="AC13" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="AD13" s="2">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="9">
-        <v>5.12</v>
-      </c>
-      <c r="C14" s="9">
-        <v>14.94</v>
-      </c>
-      <c r="D14" s="9">
-        <v>11.5</v>
-      </c>
-      <c r="E14" s="9">
-        <v>4.33</v>
-      </c>
-      <c r="F14" s="9">
-        <v>0.7</v>
-      </c>
-      <c r="G14" s="9">
-        <v>36.369999999999997</v>
-      </c>
-      <c r="H14" s="9">
-        <v>2.5099999999999998</v>
-      </c>
-      <c r="I14" s="9">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="J14" s="9">
-        <v>0.22</v>
-      </c>
-      <c r="K14" s="9">
-        <v>108.35</v>
-      </c>
-      <c r="L14" s="9">
-        <v>72.260000000000005</v>
-      </c>
+    <row r="14" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
       <c r="M14" s="9"/>
       <c r="N14" s="9"/>
       <c r="O14" s="9"/>
-      <c r="P14" s="9">
-        <v>5.8</v>
-      </c>
-      <c r="Q14" s="11">
-        <v>346.33</v>
-      </c>
-      <c r="R14" s="9">
-        <v>30.1</v>
-      </c>
-      <c r="S14" s="9">
-        <v>82.43</v>
-      </c>
-      <c r="T14" s="9">
-        <v>1019.25</v>
-      </c>
-      <c r="U14" s="9">
-        <v>464.6</v>
-      </c>
-      <c r="V14" s="2"/>
-      <c r="W14" s="2"/>
-      <c r="X14" s="2">
-        <v>20</v>
-      </c>
-      <c r="Y14" s="2">
-        <v>10</v>
-      </c>
-      <c r="Z14" s="2">
-        <v>50</v>
-      </c>
-      <c r="AA14" s="2">
-        <v>120</v>
-      </c>
-      <c r="AB14" s="2">
-        <v>125</v>
-      </c>
-      <c r="AC14" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="AD14" s="2">
-        <v>250</v>
-      </c>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
     </row>
-    <row r="15" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="9">
-        <v>0</v>
-      </c>
-      <c r="C15" s="9">
-        <v>0</v>
-      </c>
-      <c r="D15" s="9">
-        <v>0</v>
-      </c>
-      <c r="E15" s="9">
-        <v>0</v>
-      </c>
-      <c r="F15" s="9">
-        <v>0</v>
-      </c>
-      <c r="G15" s="9">
-        <v>0</v>
-      </c>
-      <c r="H15" s="9">
-        <v>0</v>
-      </c>
-      <c r="I15" s="9">
-        <v>0</v>
-      </c>
-      <c r="J15" s="9">
-        <v>0</v>
-      </c>
-      <c r="K15" s="9">
-        <v>89.14</v>
-      </c>
-      <c r="L15" s="9">
-        <v>50.28</v>
-      </c>
+    <row r="15" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
       <c r="M15" s="9"/>
       <c r="N15" s="9"/>
       <c r="O15" s="9"/>
-      <c r="P15" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="11">
-        <v>0</v>
-      </c>
-      <c r="R15" s="9">
-        <v>0</v>
-      </c>
-      <c r="S15" s="9">
-        <v>0</v>
-      </c>
-      <c r="T15" s="9">
-        <v>0</v>
-      </c>
-      <c r="U15" s="9">
-        <v>0</v>
-      </c>
-      <c r="V15" s="2"/>
-      <c r="W15" s="2"/>
-      <c r="X15" s="2">
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+    </row>
+    <row r="16" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+    </row>
+    <row r="17" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1">
         <v>20</v>
       </c>
-      <c r="Y15" s="2">
+      <c r="V17" s="1">
         <v>10</v>
       </c>
-      <c r="Z15" s="2">
+      <c r="W17" s="1">
         <v>50</v>
       </c>
-      <c r="AA15" s="2">
+      <c r="X17" s="1">
         <v>120</v>
       </c>
-      <c r="AB15" s="2">
+      <c r="Y17" s="1">
         <v>125</v>
       </c>
-      <c r="AC15" s="2">
+      <c r="Z17" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD15" s="2">
+      <c r="AA17" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="16" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="9">
-        <v>54.79</v>
-      </c>
-      <c r="C16" s="9">
-        <v>54.66</v>
-      </c>
-      <c r="D16" s="9">
-        <v>54.66</v>
-      </c>
-      <c r="E16" s="9">
-        <v>54.66</v>
-      </c>
-      <c r="F16" s="9">
-        <v>54.44</v>
-      </c>
-      <c r="G16" s="9">
-        <v>54.75</v>
-      </c>
-      <c r="H16" s="9">
-        <v>54.76</v>
-      </c>
-      <c r="I16" s="9">
-        <v>54.76</v>
-      </c>
-      <c r="J16" s="9">
-        <v>54.76</v>
-      </c>
-      <c r="K16" s="9">
-        <v>55.02</v>
-      </c>
-      <c r="L16" s="9">
-        <v>55.01</v>
-      </c>
-      <c r="M16" s="9">
-        <v>0</v>
-      </c>
-      <c r="N16" s="9">
-        <v>0</v>
-      </c>
-      <c r="O16" s="9">
-        <v>0</v>
-      </c>
-      <c r="P16" s="9">
-        <v>55.39</v>
-      </c>
-      <c r="Q16" s="9">
-        <v>55.39</v>
-      </c>
-      <c r="R16" s="9">
-        <v>55.41</v>
-      </c>
-      <c r="S16" s="9">
-        <v>55.41</v>
-      </c>
-      <c r="T16" s="9">
-        <v>55.41</v>
-      </c>
-      <c r="U16" s="9">
-        <v>55.37</v>
-      </c>
-      <c r="V16" s="2"/>
-      <c r="W16" s="2"/>
-      <c r="X16" s="2">
+    <row r="18" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1">
         <v>20</v>
       </c>
-      <c r="Y16" s="2">
+      <c r="V18" s="1">
         <v>10</v>
       </c>
-      <c r="Z16" s="2">
+      <c r="W18" s="1">
         <v>50</v>
       </c>
-      <c r="AA16" s="2">
+      <c r="X18" s="1">
         <v>120</v>
       </c>
-      <c r="AB16" s="2">
+      <c r="Y18" s="1">
         <v>125</v>
       </c>
-      <c r="AC16" s="2">
+      <c r="Z18" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD16" s="2">
+      <c r="AA18" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="17" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="11">
-        <v>30</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="11">
+    <row r="19" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1">
+        <v>20</v>
+      </c>
+      <c r="V19" s="1">
+        <v>10</v>
+      </c>
+      <c r="W19" s="1">
         <v>50</v>
       </c>
-      <c r="E17" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="J17" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K17" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="L17" s="11">
-        <v>65</v>
-      </c>
-      <c r="M17" s="11">
-        <v>15</v>
-      </c>
-      <c r="N17" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="O17" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="P17" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q17" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="R17" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="S17" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="T17" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="U17" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="V17" s="2"/>
-      <c r="W17" s="2"/>
-      <c r="X17" s="2">
+      <c r="X19" s="1">
+        <v>120</v>
+      </c>
+      <c r="Y19" s="1">
+        <v>125</v>
+      </c>
+      <c r="Z19" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="AA19" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1">
         <v>20</v>
       </c>
-      <c r="Y17" s="2">
+      <c r="V20" s="1">
         <v>10</v>
       </c>
-      <c r="Z17" s="2">
+      <c r="W20" s="1">
         <v>50</v>
       </c>
-      <c r="AA17" s="2">
+      <c r="X20" s="1">
         <v>120</v>
       </c>
-      <c r="AB17" s="2">
+      <c r="Y20" s="1">
         <v>125</v>
       </c>
-      <c r="AC17" s="2">
+      <c r="Z20" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD17" s="2">
+      <c r="AA20" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="18" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="11">
-        <f>COUNTIF(B13:B13,"&gt;" &amp; B17)</f>
-        <v>0</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="11">
-        <f>COUNTIF(D13:D13,"&gt;" &amp; D17)</f>
-        <v>0</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="J18" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K18" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="L18" s="11">
-        <f>COUNTIF(L13:L13,"&gt;" &amp; L17)</f>
-        <v>0</v>
-      </c>
-      <c r="M18" s="11">
-        <f>COUNTIF(M13:M13,"&gt;" &amp; M17)</f>
-        <v>0</v>
-      </c>
-      <c r="N18" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="O18" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="P18" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q18" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="R18" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="S18" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="T18" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="U18" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="V18" s="2"/>
-      <c r="W18" s="2"/>
-      <c r="X18" s="2">
+    <row r="21" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1">
         <v>20</v>
       </c>
-      <c r="Y18" s="2">
+      <c r="V21" s="1">
         <v>10</v>
       </c>
-      <c r="Z18" s="2">
+      <c r="W21" s="1">
         <v>50</v>
       </c>
-      <c r="AA18" s="2">
+      <c r="X21" s="1">
         <v>120</v>
       </c>
-      <c r="AB18" s="2">
+      <c r="Y21" s="1">
         <v>125</v>
       </c>
-      <c r="AC18" s="2">
+      <c r="Z21" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD18" s="2">
+      <c r="AA21" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="19" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="11"/>
-      <c r="S19" s="11"/>
-      <c r="T19" s="11"/>
-      <c r="U19" s="11"/>
-      <c r="V19" s="2"/>
-      <c r="W19" s="2"/>
-      <c r="X19" s="2">
+    <row r="22" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1">
         <v>20</v>
       </c>
-      <c r="Y19" s="2">
+      <c r="V22" s="1">
         <v>10</v>
       </c>
-      <c r="Z19" s="2">
+      <c r="W22" s="1">
         <v>50</v>
       </c>
-      <c r="AA19" s="2">
+      <c r="X22" s="1">
         <v>120</v>
       </c>
-      <c r="AB19" s="2">
+      <c r="Y22" s="1">
         <v>125</v>
       </c>
-      <c r="AC19" s="2">
+      <c r="Z22" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD19" s="2">
+      <c r="AA22" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="20" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
-      <c r="R20" s="13"/>
-      <c r="S20" s="13"/>
-      <c r="T20" s="13"/>
-      <c r="U20" s="13"/>
-      <c r="V20" s="2"/>
-      <c r="W20" s="2"/>
-      <c r="X20" s="2">
+    <row r="23" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1">
         <v>20</v>
       </c>
-      <c r="Y20" s="2">
+      <c r="V23" s="1">
         <v>10</v>
       </c>
-      <c r="Z20" s="2">
+      <c r="W23" s="1">
         <v>50</v>
       </c>
-      <c r="AA20" s="2">
+      <c r="X23" s="1">
         <v>120</v>
       </c>
-      <c r="AB20" s="2">
+      <c r="Y23" s="1">
         <v>125</v>
       </c>
-      <c r="AC20" s="2">
+      <c r="Z23" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD20" s="2">
+      <c r="AA23" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13"/>
-      <c r="U21" s="13"/>
-      <c r="V21" s="2"/>
-      <c r="W21" s="2"/>
-      <c r="X21" s="2">
+    <row r="24" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="12"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1">
         <v>20</v>
       </c>
-      <c r="Y21" s="2">
+      <c r="V24" s="1">
         <v>10</v>
       </c>
-      <c r="Z21" s="2">
+      <c r="W24" s="1">
         <v>50</v>
       </c>
-      <c r="AA21" s="2">
+      <c r="X24" s="1">
         <v>120</v>
       </c>
-      <c r="AB21" s="2">
+      <c r="Y24" s="1">
         <v>125</v>
       </c>
-      <c r="AC21" s="2">
+      <c r="Z24" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD21" s="2">
+      <c r="AA24" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="13"/>
-      <c r="S22" s="13"/>
-      <c r="T22" s="13"/>
-      <c r="U22" s="13"/>
-      <c r="V22" s="2"/>
-      <c r="W22" s="2"/>
-      <c r="X22" s="2">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1">
         <v>20</v>
       </c>
-      <c r="Y22" s="2">
+      <c r="V25" s="1">
         <v>10</v>
       </c>
-      <c r="Z22" s="2">
+      <c r="W25" s="1">
         <v>50</v>
       </c>
-      <c r="AA22" s="2">
+      <c r="X25" s="1">
         <v>120</v>
       </c>
-      <c r="AB22" s="2">
+      <c r="Y25" s="1">
         <v>125</v>
       </c>
-      <c r="AC22" s="2">
+      <c r="Z25" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD22" s="2">
+      <c r="AA25" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="13"/>
-      <c r="T23" s="13"/>
-      <c r="U23" s="13"/>
-      <c r="V23" s="2"/>
-      <c r="W23" s="2"/>
-      <c r="X23" s="2">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1">
         <v>20</v>
       </c>
-      <c r="Y23" s="2">
+      <c r="V26" s="1">
         <v>10</v>
       </c>
-      <c r="Z23" s="2">
+      <c r="W26" s="1">
         <v>50</v>
       </c>
-      <c r="AA23" s="2">
+      <c r="X26" s="1">
         <v>120</v>
       </c>
-      <c r="AB23" s="2">
+      <c r="Y26" s="1">
         <v>125</v>
       </c>
-      <c r="AC23" s="2">
+      <c r="Z26" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD23" s="2">
+      <c r="AA26" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="13"/>
-      <c r="S24" s="13"/>
-      <c r="T24" s="13"/>
-      <c r="U24" s="13"/>
-      <c r="V24" s="2"/>
-      <c r="W24" s="2"/>
-      <c r="X24" s="2">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1">
         <v>20</v>
       </c>
-      <c r="Y24" s="2">
+      <c r="V27" s="1">
         <v>10</v>
       </c>
-      <c r="Z24" s="2">
+      <c r="W27" s="1">
         <v>50</v>
       </c>
-      <c r="AA24" s="2">
+      <c r="X27" s="1">
         <v>120</v>
       </c>
-      <c r="AB24" s="2">
+      <c r="Y27" s="1">
         <v>125</v>
       </c>
-      <c r="AC24" s="2">
+      <c r="Z27" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD24" s="2">
+      <c r="AA27" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="X25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1">
         <v>20</v>
       </c>
-      <c r="Y25">
+      <c r="V28" s="1">
         <v>10</v>
       </c>
-      <c r="Z25">
+      <c r="W28" s="1">
         <v>50</v>
       </c>
-      <c r="AA25">
+      <c r="X28" s="1">
         <v>120</v>
       </c>
-      <c r="AB25">
+      <c r="Y28" s="1">
         <v>125</v>
       </c>
-      <c r="AC25">
+      <c r="Z28" s="1">
         <v>1.5</v>
       </c>
-      <c r="AD25">
+      <c r="AA28" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="X26">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="U29">
         <v>20</v>
       </c>
-      <c r="Y26">
+      <c r="V29">
         <v>10</v>
       </c>
-      <c r="Z26">
+      <c r="W29">
         <v>50</v>
       </c>
-      <c r="AA26">
+      <c r="X29">
         <v>120</v>
       </c>
-      <c r="AB26">
+      <c r="Y29">
         <v>125</v>
       </c>
-      <c r="AC26">
+      <c r="Z29">
         <v>1.5</v>
       </c>
-      <c r="AD26">
+      <c r="AA29">
         <v>250</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="X27">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="U30">
         <v>20</v>
       </c>
-      <c r="Y27">
+      <c r="V30">
         <v>10</v>
       </c>
-      <c r="Z27">
+      <c r="W30">
         <v>50</v>
       </c>
-      <c r="AA27">
+      <c r="X30">
         <v>120</v>
       </c>
-      <c r="AB27">
+      <c r="Y30">
         <v>125</v>
       </c>
-      <c r="AC27">
+      <c r="Z30">
         <v>1.5</v>
       </c>
-      <c r="AD27">
+      <c r="AA30">
         <v>250</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="X28">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="U31">
         <v>20</v>
       </c>
-      <c r="Y28">
+      <c r="V31">
         <v>10</v>
       </c>
-      <c r="Z28">
+      <c r="W31">
         <v>50</v>
       </c>
-      <c r="AA28">
+      <c r="X31">
         <v>120</v>
       </c>
-      <c r="AB28">
+      <c r="Y31">
         <v>125</v>
       </c>
-      <c r="AC28">
+      <c r="Z31">
         <v>1.5</v>
       </c>
-      <c r="AD28">
+      <c r="AA31">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="U32">
+        <v>20</v>
+      </c>
+      <c r="V32">
+        <v>10</v>
+      </c>
+      <c r="W32">
+        <v>50</v>
+      </c>
+      <c r="X32">
+        <v>120</v>
+      </c>
+      <c r="Y32">
+        <v>125</v>
+      </c>
+      <c r="Z32">
+        <v>1.5</v>
+      </c>
+      <c r="AA32">
         <v>250</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A1:U1"/>
-    <mergeCell ref="A2:S2"/>
-    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="B24:R28"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A2:P2"/>
+    <mergeCell ref="Q2:R2"/>
     <mergeCell ref="A3:G3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="B20:U24"/>
+    <mergeCell ref="Q3:R3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
A lot of fixes
</commit_message>
<xml_diff>
--- a/report_template/yearly_report.xlsx
+++ b/report_template/yearly_report.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\webApp\AQM\report_template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="工作表2" sheetId="2" r:id="rId2"/>
     <sheet name="工作表3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="114210"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -258,11 +263,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_ ;[Red]\-0.00\ "/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -435,12 +440,30 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -462,6 +485,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln w="25400">
@@ -469,10 +493,12 @@
         </a:ln>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -506,20 +532,36 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$AA$5:$AA$13</c:f>
+              <c:f>監測年報表!$AA$5:$AA$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C9EB-4F1F-B685-5B655513C81B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="67474176"/>
         <c:axId val="67476864"/>
       </c:lineChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -546,14 +588,28 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>監測年報表!$AB$5:$AB$13</c:f>
+              <c:f>監測年報表!$AB$5:$AB$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C9EB-4F1F-B685-5B655513C81B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:axId val="67483136"/>
         <c:axId val="67484672"/>
       </c:scatterChart>
@@ -562,6 +618,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -579,6 +636,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -587,18 +645,22 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="67476864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="67476864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -617,6 +679,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -625,6 +688,8 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="0.00_ ;[Red]\-0.00\ " sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="67474176"/>
         <c:crosses val="autoZero"/>
@@ -637,6 +702,8 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="67484672"/>
         <c:crosses val="autoZero"/>
@@ -649,6 +716,7 @@
           <c:max val="360"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="r"/>
         <c:title>
           <c:tx>
@@ -666,6 +734,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -674,6 +743,8 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="67483136"/>
         <c:crosses val="max"/>
@@ -693,9 +764,11 @@
           <c:h val="0.10486891385767791"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -706,8 +779,18 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -754,6 +837,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln w="25400">
@@ -761,10 +845,12 @@
         </a:ln>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -798,13 +884,19 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$B$5:$B$13</c:f>
+              <c:f>監測年報表!$B$5:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2AD0-4739-A4A8-CE2C3A892878}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -833,10 +925,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$AI$5:$AI$13</c:f>
+              <c:f>監測年報表!$AI$5:$AI$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -864,13 +956,29 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2AD0-4739-A4A8-CE2C3A892878}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="67597824"/>
         <c:axId val="67608576"/>
       </c:lineChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -897,14 +1005,28 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>監測年報表!$AB$5:$AB$13</c:f>
+              <c:f>監測年報表!$AB$5:$AB$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2AD0-4739-A4A8-CE2C3A892878}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:axId val="67610496"/>
         <c:axId val="67612032"/>
       </c:scatterChart>
@@ -913,6 +1035,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -930,6 +1053,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -938,18 +1062,22 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="67608576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="67608576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -968,6 +1096,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -976,6 +1105,8 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="0.00_ ;[Red]\-0.00\ " sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="67597824"/>
         <c:crosses val="autoZero"/>
@@ -988,6 +1119,8 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="67612032"/>
         <c:crosses val="autoZero"/>
@@ -1000,6 +1133,7 @@
           <c:max val="360"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="r"/>
         <c:title>
           <c:tx>
@@ -1017,6 +1151,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -1025,6 +1160,8 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="67610496"/>
         <c:crosses val="max"/>
@@ -1044,9 +1181,11 @@
           <c:h val="0.10486891385767791"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1057,8 +1196,18 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1105,6 +1254,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln w="25400">
@@ -1112,10 +1262,12 @@
         </a:ln>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1149,13 +1301,19 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$F$5:$F$13</c:f>
+              <c:f>監測年報表!$F$5:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A912-4ACF-85DE-3D0B1A2773AF}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1184,10 +1342,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$AJ$5:$AJ$13</c:f>
+              <c:f>監測年報表!$AJ$5:$AJ$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -1215,13 +1373,29 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A912-4ACF-85DE-3D0B1A2773AF}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="68245376"/>
         <c:axId val="68264320"/>
       </c:lineChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -1248,14 +1422,28 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>監測年報表!$AB$5:$AB$13</c:f>
+              <c:f>監測年報表!$AB$5:$AB$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A912-4ACF-85DE-3D0B1A2773AF}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:axId val="68266240"/>
         <c:axId val="68268032"/>
       </c:scatterChart>
@@ -1264,6 +1452,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1281,6 +1470,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -1289,18 +1479,22 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="68264320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="68264320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -1319,6 +1513,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -1327,6 +1522,8 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="0.00_ ;[Red]\-0.00\ " sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="68245376"/>
         <c:crosses val="autoZero"/>
@@ -1339,6 +1536,8 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="68268032"/>
         <c:crosses val="autoZero"/>
@@ -1351,6 +1550,7 @@
           <c:max val="360"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="r"/>
         <c:title>
           <c:tx>
@@ -1368,6 +1568,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -1376,6 +1577,8 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="68266240"/>
         <c:crosses val="max"/>
@@ -1395,9 +1598,11 @@
           <c:h val="0.10486891385767791"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1408,8 +1613,18 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1456,6 +1671,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln w="25400">
@@ -1463,10 +1679,12 @@
         </a:ln>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1500,13 +1718,19 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$D$5:$D$13</c:f>
+              <c:f>監測年報表!$D$5:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-748C-4772-8ED1-644EA8FC70A2}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1535,10 +1759,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$AK$5:$AK$13</c:f>
+              <c:f>監測年報表!$AK$5:$AK$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>50</c:v>
                 </c:pt>
@@ -1566,13 +1790,29 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-748C-4772-8ED1-644EA8FC70A2}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="69228800"/>
         <c:axId val="69239552"/>
       </c:lineChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -1599,14 +1839,28 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>監測年報表!$AB$5:$AB$13</c:f>
+              <c:f>監測年報表!$AB$5:$AB$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-748C-4772-8ED1-644EA8FC70A2}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:axId val="69241472"/>
         <c:axId val="69255552"/>
       </c:scatterChart>
@@ -1615,6 +1869,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1632,6 +1887,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -1640,18 +1896,22 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="69239552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="69239552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -1670,6 +1930,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -1678,6 +1939,8 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="0.00_ ;[Red]\-0.00\ " sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="69228800"/>
         <c:crosses val="autoZero"/>
@@ -1690,6 +1953,8 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="69255552"/>
         <c:crosses val="autoZero"/>
@@ -1702,6 +1967,7 @@
           <c:max val="360"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="r"/>
         <c:title>
           <c:tx>
@@ -1719,6 +1985,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -1727,6 +1994,8 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="69241472"/>
         <c:crosses val="max"/>
@@ -1746,9 +2015,11 @@
           <c:h val="0.10486891385767791"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1759,8 +2030,18 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1775,7 +2056,7 @@
               <a:rPr lang="zh-TW" altLang="en-US" sz="1800">
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>大城站  周界臭氧  平均值趨勢圖</a:t>
+              <a:t>大城站  臭氧  平均值趨勢圖</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="zh-TW" altLang="en-US" sz="1000">
@@ -1807,6 +2088,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln w="25400">
@@ -1814,10 +2096,12 @@
         </a:ln>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1851,13 +2135,19 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$G$5:$G$13</c:f>
+              <c:f>監測年報表!$G$5:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-91FA-4ED8-930F-04F17A1D87C0}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1886,10 +2176,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$AL$5:$AL$13</c:f>
+              <c:f>監測年報表!$AL$5:$AL$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>120</c:v>
                 </c:pt>
@@ -1917,13 +2207,29 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-91FA-4ED8-930F-04F17A1D87C0}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="70331776"/>
         <c:axId val="70346624"/>
       </c:lineChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -1950,14 +2256,28 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>監測年報表!$AB$5:$AB$13</c:f>
+              <c:f>監測年報表!$AB$5:$AB$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-91FA-4ED8-930F-04F17A1D87C0}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:axId val="70348800"/>
         <c:axId val="70350336"/>
       </c:scatterChart>
@@ -1966,6 +2286,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1983,6 +2304,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -1991,18 +2313,22 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="70346624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="70346624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -2021,6 +2347,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -2029,6 +2356,8 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="0.00_ ;[Red]\-0.00\ " sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="70331776"/>
         <c:crosses val="autoZero"/>
@@ -2041,6 +2370,8 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="70350336"/>
         <c:crosses val="autoZero"/>
@@ -2053,6 +2384,7 @@
           <c:max val="360"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="r"/>
         <c:title>
           <c:tx>
@@ -2070,6 +2402,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -2078,6 +2411,8 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="70348800"/>
         <c:crosses val="max"/>
@@ -2097,9 +2432,11 @@
           <c:h val="0.10486891385767791"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2110,8 +2447,18 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2126,7 +2473,7 @@
               <a:rPr lang="zh-TW" altLang="en-US" sz="1800">
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>大城站  周界</a:t>
+              <a:t>大城站  </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" altLang="en-US" sz="1800">
@@ -2170,6 +2517,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln w="25400">
@@ -2177,10 +2525,12 @@
         </a:ln>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2214,13 +2564,19 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$Z$5:$Z$13</c:f>
+              <c:f>監測年報表!$Z$5:$Z$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-69EE-4D2A-98F4-C225A6E36D67}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2249,10 +2605,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$AM$5:$AM$13</c:f>
+              <c:f>監測年報表!$AM$5:$AM$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>125</c:v>
                 </c:pt>
@@ -2280,13 +2636,29 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-69EE-4D2A-98F4-C225A6E36D67}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="70664576"/>
         <c:axId val="70666880"/>
       </c:lineChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -2313,14 +2685,28 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>監測年報表!$AB$5:$AB$13</c:f>
+              <c:f>監測年報表!$AB$5:$AB$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-69EE-4D2A-98F4-C225A6E36D67}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:axId val="70673152"/>
         <c:axId val="70674688"/>
       </c:scatterChart>
@@ -2329,6 +2715,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -2346,6 +2733,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -2354,18 +2742,22 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="70666880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="70666880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -2384,6 +2776,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -2392,6 +2785,8 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="0.00_ ;[Red]\-0.00\ " sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="70664576"/>
         <c:crosses val="autoZero"/>
@@ -2404,6 +2799,8 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="70674688"/>
         <c:crosses val="autoZero"/>
@@ -2416,6 +2813,7 @@
           <c:max val="360"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="r"/>
         <c:title>
           <c:tx>
@@ -2433,6 +2831,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -2441,6 +2840,8 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="70673152"/>
         <c:crosses val="max"/>
@@ -2460,9 +2861,11 @@
           <c:h val="0.10486891385767791"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2473,8 +2876,18 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2521,6 +2934,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln w="25400">
@@ -2528,10 +2942,12 @@
         </a:ln>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2565,13 +2981,19 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$J$5:$J$13</c:f>
+              <c:f>監測年報表!$J$5:$J$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CF86-4EF7-9015-229EB54118DB}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2600,10 +3022,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$AN$5:$AN$13</c:f>
+              <c:f>監測年報表!$AN$5:$AN$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1.5</c:v>
                 </c:pt>
@@ -2631,13 +3053,29 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CF86-4EF7-9015-229EB54118DB}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="71045888"/>
         <c:axId val="71048192"/>
       </c:lineChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -2664,14 +3102,28 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>監測年報表!$AB$5:$AB$13</c:f>
+              <c:f>監測年報表!$AB$5:$AB$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-CF86-4EF7-9015-229EB54118DB}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:axId val="71066752"/>
         <c:axId val="71068288"/>
       </c:scatterChart>
@@ -2680,6 +3132,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -2697,6 +3150,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -2705,18 +3159,22 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="71048192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="71048192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -2735,6 +3193,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -2743,6 +3202,8 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="0.00_ ;[Red]\-0.00\ " sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="71045888"/>
         <c:crosses val="autoZero"/>
@@ -2755,6 +3216,8 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="71068288"/>
         <c:crosses val="autoZero"/>
@@ -2767,6 +3230,7 @@
           <c:max val="360"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="r"/>
         <c:title>
           <c:tx>
@@ -2784,6 +3248,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -2792,6 +3257,8 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="71066752"/>
         <c:crosses val="max"/>
@@ -2811,9 +3278,11 @@
           <c:h val="0.10486891385767791"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2824,8 +3293,18 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2884,6 +3363,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln w="25400">
@@ -2891,10 +3371,12 @@
         </a:ln>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2928,13 +3410,19 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$X$5:$X$13</c:f>
+              <c:f>監測年報表!$X$5:$X$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CCC5-464C-B7CD-810F9FD1B4DD}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2963,10 +3451,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>監測年報表!$AO$5:$AO$13</c:f>
+              <c:f>監測年報表!$AO$5:$AO$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>250</c:v>
                 </c:pt>
@@ -2994,13 +3482,29 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CCC5-464C-B7CD-810F9FD1B4DD}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="71107712"/>
         <c:axId val="71110016"/>
       </c:lineChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -3027,14 +3531,28 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>監測年報表!$AB$5:$AB$13</c:f>
+              <c:f>監測年報表!$AB$5:$AB$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-CCC5-464C-B7CD-810F9FD1B4DD}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:axId val="71120384"/>
         <c:axId val="71121920"/>
       </c:scatterChart>
@@ -3043,6 +3561,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -3060,6 +3579,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -3068,18 +3588,22 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="71110016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="71110016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -3098,6 +3622,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -3106,6 +3631,8 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="0.00_ ;[Red]\-0.00\ " sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="71107712"/>
         <c:crosses val="autoZero"/>
@@ -3118,6 +3645,8 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:crossAx val="71121920"/>
         <c:crosses val="autoZero"/>
@@ -3130,6 +3659,7 @@
           <c:max val="360"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="r"/>
         <c:title>
           <c:tx>
@@ -3147,6 +3677,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -3155,6 +3686,8 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="##0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="71120384"/>
         <c:crosses val="max"/>
@@ -3174,9 +3707,11 @@
           <c:h val="0.10486891385767791"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -3448,7 +3983,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3490,7 +4025,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3522,9 +4057,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3556,6 +4109,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3731,19 +4302,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="41" width="11.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -3788,7 +4359,7 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
     </row>
-    <row r="2" spans="1:41" ht="20.100000000000001" customHeight="1">
+    <row r="2" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
@@ -3833,7 +4404,7 @@
       <c r="AN2" s="1"/>
       <c r="AO2" s="1"/>
     </row>
-    <row r="3" spans="1:41" ht="20.100000000000001" customHeight="1">
+    <row r="3" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>2</v>
       </c>
@@ -3865,7 +4436,7 @@
       <c r="AN3" s="1"/>
       <c r="AO3" s="1"/>
     </row>
-    <row r="4" spans="1:41" ht="35.1" customHeight="1">
+    <row r="4" spans="1:41" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -3986,7 +4557,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:41" ht="20.100000000000001" customHeight="1">
+    <row r="5" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
@@ -4045,7 +4616,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:41" ht="20.100000000000001" customHeight="1">
+    <row r="6" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>27</v>
       </c>
@@ -4104,7 +4675,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:41" ht="20.100000000000001" customHeight="1">
+    <row r="7" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>28</v>
       </c>
@@ -4163,7 +4734,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="1:41" ht="20.100000000000001" customHeight="1">
+    <row r="8" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>29</v>
       </c>
@@ -4222,7 +4793,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="9" spans="1:41" ht="20.100000000000001" customHeight="1">
+    <row r="9" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>30</v>
       </c>
@@ -4281,7 +4852,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="10" spans="1:41" ht="20.100000000000001" customHeight="1">
+    <row r="10" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>31</v>
       </c>
@@ -4340,7 +4911,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:41" ht="20.100000000000001" customHeight="1">
+    <row r="11" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>32</v>
       </c>
@@ -4399,7 +4970,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="1:41" ht="20.100000000000001" customHeight="1">
+    <row r="12" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>33</v>
       </c>
@@ -4444,7 +5015,7 @@
       <c r="AN12" s="1"/>
       <c r="AO12" s="1"/>
     </row>
-    <row r="13" spans="1:41" ht="20.100000000000001" customHeight="1">
+    <row r="13" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>34</v>
       </c>
@@ -4503,7 +5074,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="14" spans="1:41" ht="20.100000000000001" customHeight="1">
+    <row r="14" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>35</v>
       </c>
@@ -4548,7 +5119,7 @@
       <c r="AN14" s="1"/>
       <c r="AO14" s="1"/>
     </row>
-    <row r="15" spans="1:41" ht="20.100000000000001" customHeight="1">
+    <row r="15" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>36</v>
       </c>
@@ -4593,7 +5164,7 @@
       <c r="AN15" s="1"/>
       <c r="AO15" s="1"/>
     </row>
-    <row r="16" spans="1:41" ht="20.100000000000001" customHeight="1">
+    <row r="16" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>37</v>
       </c>
@@ -4638,7 +5209,7 @@
       <c r="AN16" s="1"/>
       <c r="AO16" s="1"/>
     </row>
-    <row r="17" spans="1:41" ht="20.100000000000001" customHeight="1">
+    <row r="17" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
@@ -4697,7 +5268,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="18" spans="1:41" ht="20.100000000000001" customHeight="1">
+    <row r="18" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
@@ -4756,7 +5327,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="19" spans="1:41" ht="20.100000000000001" customHeight="1">
+    <row r="19" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
@@ -4815,7 +5386,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="20" spans="1:41" ht="20.100000000000001" customHeight="1">
+    <row r="20" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>38</v>
       </c>
@@ -4874,7 +5445,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="21" spans="1:41" s="16" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="21" spans="1:41" s="16" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>55</v>
       </c>
@@ -4995,7 +5566,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="22" spans="1:41" s="16" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="22" spans="1:41" s="16" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>57</v>
       </c>
@@ -5069,7 +5640,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="23" spans="1:41" ht="20.100000000000001" customHeight="1">
+    <row r="23" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -5126,7 +5697,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="24" spans="1:41" ht="20.100000000000001" customHeight="1">
+    <row r="24" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>23</v>
       </c>
@@ -5185,7 +5756,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="1:41">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="19"/>
       <c r="C25" s="19"/>
@@ -5242,7 +5813,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="26" spans="1:41">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A26" s="18"/>
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
@@ -5299,7 +5870,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="27" spans="1:41">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
       <c r="B27" s="19"/>
       <c r="C27" s="19"/>
@@ -5356,7 +5927,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="28" spans="1:41">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
@@ -5413,7 +5984,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="29" spans="1:41">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
       <c r="AI29">
         <v>20</v>
       </c>
@@ -5436,7 +6007,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="30" spans="1:41">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
       <c r="AI30">
         <v>20</v>
       </c>
@@ -5459,7 +6030,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="31" spans="1:41">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
       <c r="AI31">
         <v>20</v>
       </c>
@@ -5482,7 +6053,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="32" spans="1:41">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
       <c r="AI32">
         <v>20</v>
       </c>
@@ -5524,12 +6095,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5537,12 +6108,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>